<commit_message>
added fib 4.c (gold)
</commit_message>
<xml_diff>
--- a/pytester/pytester/data4test/fib/fib_results.xlsx
+++ b/pytester/pytester/data4test/fib/fib_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan.Vekhov\WORK\algo\AlgoOtus\pytester\pytester\data4test\fib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841DE58B-BC5F-46F0-B6FF-91DDA1AC86EA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37004369-E98F-4033-95C6-7A68D8DD215F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A88667C6-E2DC-46F9-B182-1A36D3E3DF7E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="61">
   <si>
     <t>------------------------------------------------------------------------</t>
   </si>
@@ -126,27 +126,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>fib_iteration_4b,test.0.in,0,True,0.003152,2020-02-07 17:59:08.706976</t>
-  </si>
-  <si>
-    <t>fib_iteration_4b,test.1.in,1,True,0.0078031,2020-02-07 17:59:08.714354</t>
-  </si>
-  <si>
-    <t>fib_iteration_4b,test.2.in,2,True,0.0032145,2020-02-07 17:59:08.717425</t>
-  </si>
-  <si>
-    <t>fib_iteration_4b,test.3.in,3,True,0.0032896,2020-02-07 17:59:08.721369</t>
-  </si>
-  <si>
-    <t>fib_iteration_4b,test.4.in,4,True,0.002602,2020-02-07 17:59:08.724383</t>
-  </si>
-  <si>
-    <t>fib_iteration_4b,test.5.in,5,True,0.005845,2020-02-07 17:59:08.730399</t>
-  </si>
-  <si>
-    <t>fib_iteration_4b,test.6.in,6,True,0.0030685,2020-02-07 17:59:08.733405</t>
-  </si>
-  <si>
     <t>fib_iteration_4b</t>
   </si>
   <si>
@@ -190,6 +169,51 @@
   </si>
   <si>
     <t>2020-02-07 17:59:08.733405</t>
+  </si>
+  <si>
+    <t>0.0018188</t>
+  </si>
+  <si>
+    <t>0.0025526</t>
+  </si>
+  <si>
+    <t>0.0061877</t>
+  </si>
+  <si>
+    <t>0.0050125</t>
+  </si>
+  <si>
+    <t>0.001975</t>
+  </si>
+  <si>
+    <t>0.0049472</t>
+  </si>
+  <si>
+    <t>0.0033072</t>
+  </si>
+  <si>
+    <t>fib_gold_4c</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.0.in,0,True,0.0018188,2020-02-07 18:10:27.938622</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.1.in,1,True,0.0025526,2020-02-07 18:10:27.941126</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.2.in,2,True,0.0061877,2020-02-07 18:10:27.947649</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.3.in,3,True,0.0050125,2020-02-07 18:10:27.952662</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.4.in,4,True,0.001975,2020-02-07 18:10:27.954668</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.5.in,5,True,0.0049472,2020-02-07 18:10:27.959682</t>
+  </si>
+  <si>
+    <t>fib_gold_4c,test.6.in,6,True,0.0033072,2020-02-07 18:10:27.963061</t>
   </si>
 </sst>
 </file>
@@ -207,7 +231,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFA9B7C6"/>
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="204"/>
@@ -241,10 +264,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,20 +582,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9317D8-9669-469A-A782-377D8428918D}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -584,7 +609,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -595,7 +623,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -606,7 +637,10 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -617,7 +651,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -628,7 +665,10 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -639,7 +679,10 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -650,7 +693,10 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -661,11 +707,14 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -830,197 +879,192 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>32</v>
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>33</v>
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>35</v>
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>36</v>
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>37</v>
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
-      </c>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>47</v>
-      </c>
-      <c r="F38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40">
-        <v>6</v>
-      </c>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>51</v>
-      </c>
-      <c r="F40" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>